<commit_message>
update: excel tracking log
</commit_message>
<xml_diff>
--- a/FYP-ProgressTrack.xlsx
+++ b/FYP-ProgressTrack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamlotfi/Desktop/FYP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E94CDC87-6C9A-DD44-A781-92854993926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD60CA-A4F4-344E-A1EA-10A5313FF413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{18A0949A-A941-4942-A929-12DEA1FC6C68}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update: fyp1 docs link in excel
</commit_message>
<xml_diff>
--- a/FYP-ProgressTrack.xlsx
+++ b/FYP-ProgressTrack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamlotfi/Desktop/FYP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD60CA-A4F4-344E-A1EA-10A5313FF413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678DE836-5A43-A344-8F25-D6202063BA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{18A0949A-A941-4942-A929-12DEA1FC6C68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Task ID</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Organize &amp; push all docs to GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link to FYP1 Report: </t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1rVbWoatZkmNisgtaDAgxFU5iTkoyqhf5CVGZ_pejgjM/edit?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65616974-8326-BB45-B75A-9E24D54465EB}">
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,9 +638,11 @@
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="90.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,8 +661,14 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -664,7 +678,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -680,7 +694,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -696,7 +710,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -712,7 +726,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -728,7 +742,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -744,7 +758,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -760,7 +774,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -776,7 +790,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -792,7 +806,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
@@ -808,7 +822,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
@@ -818,7 +832,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
@@ -834,7 +848,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
@@ -850,7 +864,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>